<commit_message>
measures and clean up of scope data
</commit_message>
<xml_diff>
--- a/simulations/motorMålinger.xlsx
+++ b/simulations/motorMålinger.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ditte\aauRepo\esd7\3Dprinter-BLDC-control\simulations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ditte\aauRepo\esd7_git\3Dprinter-BLDC-control\simulations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{240AB953-539C-4908-A90E-C3085ECBF252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{088C6AB1-27E1-4465-8F1A-28FB8BDE22F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1435,7 +1435,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-DK"/>
+          <a:endParaRPr lang="da-DK"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4219,8 +4219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C31" zoomScale="71" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="T64" sqref="T64"/>
+    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="71" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
back calc for wrong measures. 1order system calc
</commit_message>
<xml_diff>
--- a/simulations/motorMålinger.xlsx
+++ b/simulations/motorMålinger.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ditte\aauRepo\esd7_git\3Dprinter-BLDC-control\simulations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{499FB6D5-3A3E-467D-9481-2289235F5FA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A739ECAD-14AA-4BE4-99C3-B02E86D7E388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,30 +36,8 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="77">
   <si>
     <t>From data sheet:</t>
   </si>
@@ -124,9 +102,6 @@
     <t>avg Kt</t>
   </si>
   <si>
-    <t>better Kt</t>
-  </si>
-  <si>
     <t>Measurement 1 for K_e</t>
   </si>
   <si>
@@ -170,18 +145,6 @@
   </si>
   <si>
     <t>estimate R</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>Måling af J</t>
-  </si>
-  <si>
-    <t>Tidskonstant</t>
-  </si>
-  <si>
-    <t>Estimeret J</t>
   </si>
   <si>
     <t>MÅLT R</t>
@@ -315,7 +278,7 @@
     <numFmt numFmtId="164" formatCode="0.000E+00"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -346,6 +309,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF444444"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -361,7 +330,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -401,15 +370,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -423,13 +383,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -441,15 +394,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -463,7 +407,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -474,15 +418,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -967,8 +916,13 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>B_rad/s_GEAR</a:t>
+              <a:t>B_rad/s</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> outer</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1055,43 +1009,7 @@
             </c:spPr>
             <c:trendlineType val="linear"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="3.0224846894138232E-2"/>
-                  <c:y val="-0.12667395742198892"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-DK"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
+            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -1210,6 +1128,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="da-DK"/>
+                  <a:t>rad/s</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-DK"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1272,6 +1245,69 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="da-DK"/>
+                  <a:t>Nm</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="3.7269811559350774E-2"/>
+              <c:y val="0.37627704868907896"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-DK"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3618,16 +3654,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>577195</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>48582</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>166768</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>149253</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>669270</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>48581</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>599574</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>149252</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3654,16 +3690,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>473075</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>181427</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>31853</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>48468</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>299358</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>125723</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>12699</xdr:rowOff>
+      <xdr:rowOff>38755</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3691,15 +3727,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>307975</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>408646</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>71399</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>548346</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>52349</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4047,7 +4083,7 @@
   <dimension ref="B2:D34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4058,156 +4094,156 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B2" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B5" s="5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D5" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D6" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B12" s="5" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B22" s="5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B25" s="5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B31" s="5" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -4219,8 +4255,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C9" zoomScale="71" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="W46" sqref="W46"/>
+    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4232,10 +4268,12 @@
     <col min="6" max="6" width="12.7265625" customWidth="1"/>
     <col min="7" max="7" width="12.54296875" customWidth="1"/>
     <col min="8" max="9" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.1796875" customWidth="1"/>
     <col min="12" max="12" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="1.81640625" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
@@ -4298,7 +4336,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I11">
         <v>0.09</v>
@@ -4332,13 +4370,10 @@
       <c r="J12" t="s">
         <v>20</v>
       </c>
-      <c r="K12" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B13" s="1">
         <v>3.9999999999999998E-7</v>
@@ -4356,30 +4391,27 @@
       <c r="G13">
         <v>0.4</v>
       </c>
-      <c r="H13" s="13">
+      <c r="H13" s="10">
         <f>G13*$I$11</f>
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="I13" s="13">
+      <c r="I13" s="10">
         <f>H13/F13</f>
         <v>0.17733990147783249</v>
       </c>
-      <c r="J13" s="5">
+      <c r="J13" s="13">
         <f>AVERAGE(I13:I22)</f>
         <v>0.22058002850880359</v>
       </c>
-      <c r="K13" s="5">
-        <f>AVERAGE(I14:I21)</f>
-        <v>0.22420972186431889</v>
-      </c>
+      <c r="K13" s="13"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" s="2">
         <f>G25</f>
-        <v>2.8</v>
+        <v>3.5714285714285716</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -4390,22 +4422,22 @@
       <c r="G14">
         <v>0.95</v>
       </c>
-      <c r="H14" s="13">
-        <f t="shared" ref="H14:H22" si="0">G14*$I$11</f>
+      <c r="H14" s="10">
+        <f>G14*$I$11</f>
         <v>8.5499999999999993E-2</v>
       </c>
-      <c r="I14" s="13">
-        <f t="shared" ref="I14:I22" si="1">H14/F14</f>
+      <c r="I14" s="10">
+        <f t="shared" ref="I14:I22" si="0">H14/F14</f>
         <v>0.24289772727272727</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" s="6">
         <f>B13*B14</f>
-        <v>1.1199999999999999E-6</v>
+        <v>1.4285714285714286E-6</v>
       </c>
       <c r="E15">
         <v>1.5</v>
@@ -4416,12 +4448,12 @@
       <c r="G15">
         <v>1.25</v>
       </c>
-      <c r="H15" s="13">
+      <c r="H15" s="10">
+        <f t="shared" ref="H14:H22" si="1">G15*$I$11</f>
+        <v>0.11249999999999999</v>
+      </c>
+      <c r="I15" s="10">
         <f t="shared" si="0"/>
-        <v>0.11249999999999999</v>
-      </c>
-      <c r="I15" s="13">
-        <f t="shared" si="1"/>
         <v>0.2236580516898608</v>
       </c>
     </row>
@@ -4435,16 +4467,16 @@
       <c r="G16">
         <v>1.5</v>
       </c>
-      <c r="H16" s="13">
+      <c r="H16" s="10">
+        <f t="shared" si="1"/>
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="I16" s="10">
         <f t="shared" si="0"/>
-        <v>0.13500000000000001</v>
-      </c>
-      <c r="I16" s="13">
-        <f t="shared" si="1"/>
         <v>0.2099533437013997</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
       <c r="E17">
         <v>2.5</v>
       </c>
@@ -4454,18 +4486,18 @@
       <c r="G17">
         <v>1.75</v>
       </c>
-      <c r="H17" s="13">
+      <c r="H17" s="10">
+        <f t="shared" si="1"/>
+        <v>0.1575</v>
+      </c>
+      <c r="I17" s="10">
         <f t="shared" si="0"/>
-        <v>0.1575</v>
-      </c>
-      <c r="I17" s="13">
-        <f t="shared" si="1"/>
         <v>0.20723684210526316</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E18">
         <v>3</v>
@@ -4476,18 +4508,18 @@
       <c r="G18">
         <v>2.0499999999999998</v>
       </c>
-      <c r="H18" s="13">
+      <c r="H18" s="10">
+        <f t="shared" si="1"/>
+        <v>0.18449999999999997</v>
+      </c>
+      <c r="I18" s="10">
         <f t="shared" si="0"/>
-        <v>0.18449999999999997</v>
-      </c>
-      <c r="I18" s="13">
-        <f t="shared" si="1"/>
         <v>0.20965909090909088</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B19">
         <v>0.1</v>
@@ -4501,18 +4533,18 @@
       <c r="G19">
         <v>2.25</v>
       </c>
-      <c r="H19" s="13">
+      <c r="H19" s="10">
+        <f t="shared" si="1"/>
+        <v>0.20249999999999999</v>
+      </c>
+      <c r="I19" s="10">
         <f t="shared" si="0"/>
-        <v>0.20249999999999999</v>
-      </c>
-      <c r="I19" s="13">
-        <f t="shared" si="1"/>
         <v>0.2109375</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B20">
         <v>2.8000000000000001E-2</v>
@@ -4526,18 +4558,18 @@
       <c r="G20">
         <v>2.75</v>
       </c>
-      <c r="H20" s="13">
+      <c r="H20" s="10">
+        <f t="shared" si="1"/>
+        <v>0.2475</v>
+      </c>
+      <c r="I20" s="10">
         <f t="shared" si="0"/>
-        <v>0.2475</v>
-      </c>
-      <c r="I20" s="13">
-        <f t="shared" si="1"/>
         <v>0.24504950495049505</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B21" s="5">
         <v>2.8</v>
@@ -4551,18 +4583,18 @@
       <c r="G21">
         <v>2.85</v>
       </c>
-      <c r="H21" s="13">
+      <c r="H21" s="10">
+        <f t="shared" si="1"/>
+        <v>0.25650000000000001</v>
+      </c>
+      <c r="I21" s="10">
         <f t="shared" si="0"/>
-        <v>0.25650000000000001</v>
-      </c>
-      <c r="I21" s="13">
-        <f t="shared" si="1"/>
         <v>0.24428571428571427</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B22" s="7">
         <f>B19/B20</f>
@@ -4577,27 +4609,25 @@
       <c r="G22">
         <v>3</v>
       </c>
-      <c r="H22" s="13">
+      <c r="H22" s="10">
+        <f t="shared" si="1"/>
+        <v>0.27</v>
+      </c>
+      <c r="I22" s="10">
         <f t="shared" si="0"/>
-        <v>0.27</v>
-      </c>
-      <c r="I22" s="13">
-        <f t="shared" si="1"/>
         <v>0.23478260869565221</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>38</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F25" s="7"/>
-      <c r="G25" s="8">
-        <v>2.8</v>
-      </c>
-      <c r="H25" s="7" t="s">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="E25" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F25" s="14"/>
+      <c r="G25" s="15">
+        <f>B22</f>
+        <v>3.5714285714285716</v>
+      </c>
+      <c r="H25" s="14" t="s">
         <v>15</v>
       </c>
       <c r="I25" s="7">
@@ -4614,65 +4644,53 @@
       <c r="O25" s="7"/>
       <c r="P25" s="7"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>37</v>
-      </c>
-      <c r="B26">
-        <v>0.123</v>
-      </c>
-      <c r="E26" s="7" t="s">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="E26" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="F26" s="7" t="s">
+      <c r="F26" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G26" s="7" t="s">
+      <c r="G26" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="H26" s="7" t="s">
+      <c r="H26" s="14" t="s">
         <v>17</v>
       </c>
       <c r="I26" s="7" t="s">
         <v>18</v>
       </c>
       <c r="J26" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K26" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="K26" s="7" t="s">
+      <c r="L26" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="M26" s="7"/>
+      <c r="N26" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="L26" s="7" t="s">
+      <c r="O26" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="M26" s="7"/>
-      <c r="N26" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="O26" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="P26" s="7"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>39</v>
-      </c>
-      <c r="B27" s="1">
-        <f>B13</f>
-        <v>3.9999999999999998E-7</v>
-      </c>
-      <c r="E27" s="7">
+      <c r="P26" s="14"/>
+    </row>
+    <row r="27" spans="1:18" ht="16" x14ac:dyDescent="0.45">
+      <c r="B27" s="1"/>
+      <c r="E27" s="14">
         <v>0.5</v>
       </c>
-      <c r="F27" s="7">
+      <c r="F27" s="14">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="G27" s="7">
+      <c r="G27" s="14">
         <f>$G$25</f>
-        <v>2.8</v>
-      </c>
-      <c r="H27" s="7">
+        <v>3.5714285714285716</v>
+      </c>
+      <c r="H27" s="14">
         <v>9</v>
       </c>
       <c r="I27" s="7">
@@ -4684,46 +4702,41 @@
         <v>9.1851649617667661</v>
       </c>
       <c r="K27" s="8">
-        <f>(E27-G27*F27)/J27</f>
-        <v>3.7974277157991114E-2</v>
-      </c>
-      <c r="L27" s="9" cm="1">
-        <f t="array" ref="L27">AVERAGE(K28+K32:K33)</f>
-        <v>7.5958921866733753E-2</v>
+        <f>(E27-(G27*F27))/J27</f>
+        <v>3.3439013716284771E-2</v>
+      </c>
+      <c r="L27" s="9">
+        <f>AVERAGE(K27:K36)</f>
+        <v>3.5545471252835914E-2</v>
       </c>
       <c r="M27" s="7"/>
-      <c r="N27" s="7">
+      <c r="N27" s="14">
         <f>H27*2*PI()/60</f>
         <v>0.94247779607693793</v>
       </c>
-      <c r="O27" s="7">
+      <c r="O27" s="14">
         <f>(E27-G27*F27)/N27</f>
-        <v>0.37008829433635398</v>
-      </c>
-      <c r="P27" s="10">
+        <v>0.32588869299769047</v>
+      </c>
+      <c r="P27" s="5">
         <f>AVERAGE(O27:O362)</f>
-        <v>0.35992952585541321</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>40</v>
-      </c>
-      <c r="B28" s="5">
-        <f>B26*B27</f>
-        <v>4.9199999999999997E-8</v>
-      </c>
-      <c r="E28" s="7">
+        <v>0.34641772831153644</v>
+      </c>
+      <c r="R27" s="12"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B28" s="5"/>
+      <c r="E28" s="14">
         <v>1</v>
       </c>
-      <c r="F28" s="7">
+      <c r="F28" s="14">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="G28" s="7">
+      <c r="G28" s="14">
         <f t="shared" ref="G28:G36" si="2">$G$25</f>
-        <v>2.8</v>
-      </c>
-      <c r="H28" s="7">
+        <v>3.5714285714285716</v>
+      </c>
+      <c r="H28" s="14">
         <v>21</v>
       </c>
       <c r="I28" s="7">
@@ -4735,33 +4748,34 @@
         <v>21.432051577455791</v>
       </c>
       <c r="K28" s="8">
-        <f t="shared" ref="K28:K36" si="5">(E28-G28*F28)/J28</f>
-        <v>3.9212298316975418E-2</v>
+        <f t="shared" ref="K28:K36" si="5">(E28-(G28*F28))/J28</f>
+        <v>3.7160631521917779E-2</v>
       </c>
       <c r="L28" s="7"/>
       <c r="M28" s="7"/>
-      <c r="N28" s="7">
+      <c r="N28" s="14">
         <f t="shared" ref="N28:N36" si="6">H28*2*PI()/60</f>
         <v>2.1991148575128552</v>
       </c>
-      <c r="O28" s="7">
+      <c r="O28" s="14">
         <f t="shared" ref="O28:O36" si="7">(E28-G28*F28)/N28</f>
-        <v>0.38215375478408242</v>
-      </c>
-      <c r="P28" s="7"/>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="E29" s="7">
+        <v>0.36215869703563935</v>
+      </c>
+      <c r="P28" s="14"/>
+      <c r="R28" s="2"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="E29" s="14">
         <v>1.5</v>
       </c>
-      <c r="F29" s="7">
+      <c r="F29" s="14">
         <v>6.3E-2</v>
       </c>
-      <c r="G29" s="7">
+      <c r="G29" s="14">
         <f t="shared" si="2"/>
-        <v>2.8</v>
-      </c>
-      <c r="H29" s="7">
+        <v>3.5714285714285716</v>
+      </c>
+      <c r="H29" s="14">
         <v>38</v>
       </c>
       <c r="I29" s="7">
@@ -4773,33 +4787,33 @@
         <v>38.78180761634858</v>
       </c>
       <c r="K29" s="8">
-        <f>(E29-G29*F29)/J29</f>
-        <v>3.4129404515998697E-2</v>
+        <f t="shared" si="5"/>
+        <v>3.2876239617632474E-2</v>
       </c>
       <c r="L29" s="7"/>
       <c r="M29" s="7"/>
-      <c r="N29" s="7">
+      <c r="N29" s="14">
         <f t="shared" si="6"/>
         <v>3.9793506945470711</v>
       </c>
-      <c r="O29" s="7">
+      <c r="O29" s="14">
         <f t="shared" si="7"/>
-        <v>0.33261707791015682</v>
-      </c>
-      <c r="P29" s="7"/>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="E30" s="7">
+        <v>0.32040403017184194</v>
+      </c>
+      <c r="P29" s="14"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="E30" s="14">
         <v>2</v>
       </c>
-      <c r="F30" s="7">
+      <c r="F30" s="14">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="G30" s="7">
+      <c r="G30" s="14">
         <f t="shared" si="2"/>
-        <v>2.8</v>
-      </c>
-      <c r="H30" s="7">
+        <v>3.5714285714285716</v>
+      </c>
+      <c r="H30" s="14">
         <v>50</v>
       </c>
       <c r="I30" s="7">
@@ -4812,32 +4826,32 @@
       </c>
       <c r="K30" s="8">
         <f t="shared" si="5"/>
-        <v>3.551727174829631E-2</v>
+        <v>3.4504396246315225E-2</v>
       </c>
       <c r="L30" s="7"/>
       <c r="M30" s="7"/>
-      <c r="N30" s="7">
+      <c r="N30" s="14">
         <f t="shared" si="6"/>
         <v>5.2359877559829888</v>
       </c>
-      <c r="O30" s="7">
+      <c r="O30" s="14">
         <f t="shared" si="7"/>
-        <v>0.34614290263170133</v>
-      </c>
-      <c r="P30" s="7"/>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="E31" s="7">
+        <v>0.33627165833273315</v>
+      </c>
+      <c r="P30" s="14"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="E31" s="14">
         <v>2.5</v>
       </c>
-      <c r="F31" s="7">
+      <c r="F31" s="14">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="G31" s="7">
+      <c r="G31" s="14">
         <f t="shared" si="2"/>
-        <v>2.8</v>
-      </c>
-      <c r="H31" s="7">
+        <v>3.5714285714285716</v>
+      </c>
+      <c r="H31" s="14">
         <v>61</v>
       </c>
       <c r="I31" s="7">
@@ -4850,32 +4864,32 @@
       </c>
       <c r="K31" s="8">
         <f t="shared" si="5"/>
-        <v>3.6784189926407945E-2</v>
+        <v>3.5854832663763207E-2</v>
       </c>
       <c r="L31" s="7"/>
       <c r="M31" s="7"/>
-      <c r="N31" s="7">
+      <c r="N31" s="14">
         <f t="shared" si="6"/>
         <v>6.3879050622992457</v>
       </c>
-      <c r="O31" s="7">
+      <c r="O31" s="14">
         <f t="shared" si="7"/>
-        <v>0.35848998657092496</v>
-      </c>
-      <c r="P31" s="7"/>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="E32" s="7">
+        <v>0.34943269121464143</v>
+      </c>
+      <c r="P31" s="14"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="E32" s="14">
         <v>3</v>
       </c>
-      <c r="F32" s="7">
+      <c r="F32" s="14">
         <v>8.4000000000000005E-2</v>
       </c>
-      <c r="G32" s="7">
+      <c r="G32" s="14">
         <f t="shared" si="2"/>
-        <v>2.8</v>
-      </c>
-      <c r="H32" s="7">
+        <v>3.5714285714285716</v>
+      </c>
+      <c r="H32" s="14">
         <v>77</v>
       </c>
       <c r="I32" s="7">
@@ -4888,32 +4902,32 @@
       </c>
       <c r="K32" s="8">
         <f t="shared" si="5"/>
-        <v>3.5182649729600723E-2</v>
+        <v>3.4358056376563202E-2</v>
       </c>
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
-      <c r="N32" s="7">
+      <c r="N32" s="14">
         <f t="shared" si="6"/>
         <v>8.0634211442138017</v>
       </c>
-      <c r="O32" s="7">
+      <c r="O32" s="14">
         <f t="shared" si="7"/>
-        <v>0.34288175583932906</v>
-      </c>
-      <c r="P32" s="7"/>
+        <v>0.33484546468684478</v>
+      </c>
+      <c r="P32" s="14"/>
     </row>
     <row r="33" spans="5:16" x14ac:dyDescent="0.35">
-      <c r="E33" s="7">
+      <c r="E33" s="14">
         <v>3.5</v>
       </c>
-      <c r="F33" s="7">
+      <c r="F33" s="14">
         <v>9.0999999999999998E-2</v>
       </c>
-      <c r="G33" s="7">
+      <c r="G33" s="14">
         <f t="shared" si="2"/>
-        <v>2.8</v>
-      </c>
-      <c r="H33" s="7">
+        <v>3.5714285714285716</v>
+      </c>
+      <c r="H33" s="14">
         <v>83</v>
       </c>
       <c r="I33" s="7">
@@ -4926,32 +4940,32 @@
       </c>
       <c r="K33" s="8">
         <f t="shared" si="5"/>
-        <v>3.831059736991594E-2</v>
+        <v>3.7481864492013774E-2</v>
       </c>
       <c r="L33" s="7"/>
       <c r="M33" s="7"/>
-      <c r="N33" s="7">
+      <c r="N33" s="14">
         <f t="shared" si="6"/>
         <v>8.6917396749317621</v>
       </c>
-      <c r="O33" s="7">
+      <c r="O33" s="14">
         <f t="shared" si="7"/>
-        <v>0.3733659913169774</v>
-      </c>
-      <c r="P33" s="7"/>
+        <v>0.36528935733742235</v>
+      </c>
+      <c r="P33" s="14"/>
     </row>
     <row r="34" spans="5:16" x14ac:dyDescent="0.35">
-      <c r="E34" s="7">
+      <c r="E34" s="14">
         <v>4</v>
       </c>
-      <c r="F34" s="7">
+      <c r="F34" s="14">
         <v>0.105</v>
       </c>
-      <c r="G34" s="7">
+      <c r="G34" s="14">
         <f t="shared" si="2"/>
-        <v>2.8</v>
-      </c>
-      <c r="H34" s="7">
+        <v>3.5714285714285716</v>
+      </c>
+      <c r="H34" s="14">
         <v>96</v>
       </c>
       <c r="I34" s="7">
@@ -4964,32 +4978,32 @@
       </c>
       <c r="K34" s="8">
         <f t="shared" si="5"/>
-        <v>3.7825940137842705E-2</v>
+        <v>3.6999199406281651E-2</v>
       </c>
       <c r="L34" s="7"/>
       <c r="M34" s="7"/>
-      <c r="N34" s="7">
+      <c r="N34" s="14">
         <f t="shared" si="6"/>
         <v>10.053096491487338</v>
       </c>
-      <c r="O34" s="7">
+      <c r="O34" s="14">
         <f t="shared" si="7"/>
-        <v>0.3686426369366026</v>
-      </c>
-      <c r="P34" s="7"/>
+        <v>0.36058541794257537</v>
+      </c>
+      <c r="P34" s="14"/>
     </row>
     <row r="35" spans="5:16" x14ac:dyDescent="0.35">
-      <c r="E35" s="7">
+      <c r="E35" s="14">
         <v>4.5</v>
       </c>
-      <c r="F35" s="7">
+      <c r="F35" s="14">
         <v>0.11600000000000001</v>
       </c>
-      <c r="G35" s="7">
+      <c r="G35" s="14">
         <f t="shared" si="2"/>
-        <v>2.8</v>
-      </c>
-      <c r="H35" s="7">
+        <v>3.5714285714285716</v>
+      </c>
+      <c r="H35" s="14">
         <v>114</v>
       </c>
       <c r="I35" s="7">
@@ -5002,32 +5016,32 @@
       </c>
       <c r="K35" s="8">
         <f t="shared" si="5"/>
-        <v>3.5886242000402392E-2</v>
+        <v>3.5117103755902476E-2</v>
       </c>
       <c r="L35" s="7"/>
       <c r="M35" s="7"/>
-      <c r="N35" s="7">
+      <c r="N35" s="14">
         <f t="shared" si="6"/>
         <v>11.938052083641214</v>
       </c>
-      <c r="O35" s="7">
+      <c r="O35" s="14">
         <f t="shared" si="7"/>
-        <v>0.34973879915646394</v>
-      </c>
-      <c r="P35" s="7"/>
+        <v>0.34224296033294788</v>
+      </c>
+      <c r="P35" s="14"/>
     </row>
     <row r="36" spans="5:16" x14ac:dyDescent="0.35">
-      <c r="E36" s="7">
+      <c r="E36" s="14">
         <v>5</v>
       </c>
-      <c r="F36" s="7">
+      <c r="F36" s="14">
         <v>0.13</v>
       </c>
-      <c r="G36" s="7">
+      <c r="G36" s="14">
         <f t="shared" si="2"/>
-        <v>2.8</v>
-      </c>
-      <c r="H36" s="7">
+        <v>3.5714285714285716</v>
+      </c>
+      <c r="H36" s="14">
         <v>118</v>
       </c>
       <c r="I36" s="7">
@@ -5040,19 +5054,19 @@
       </c>
       <c r="K36" s="8">
         <f t="shared" si="5"/>
-        <v>3.8496120843862267E-2</v>
+        <v>3.7663374731684546E-2</v>
       </c>
       <c r="L36" s="7"/>
       <c r="M36" s="7"/>
-      <c r="N36" s="7">
+      <c r="N36" s="14">
         <f t="shared" si="6"/>
         <v>12.356931104119854</v>
       </c>
-      <c r="O36" s="7">
+      <c r="O36" s="14">
         <f t="shared" si="7"/>
-        <v>0.37517405907153906</v>
-      </c>
-      <c r="P36" s="7"/>
+        <v>0.36705831306302739</v>
+      </c>
+      <c r="P36" s="14"/>
     </row>
     <row r="38" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E38" t="s">
@@ -5061,15 +5075,15 @@
     </row>
     <row r="39" spans="5:16" x14ac:dyDescent="0.35">
       <c r="F39" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G39" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H39" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="I39" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G39" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H39" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="I39" s="21" t="s">
         <v>13</v>
       </c>
     </row>
@@ -5078,15 +5092,15 @@
         <f>J27</f>
         <v>9.1851649617667661</v>
       </c>
-      <c r="G40" s="7">
+      <c r="G40" s="19">
         <f>N27</f>
         <v>0.94247779607693793</v>
       </c>
-      <c r="H40" s="14">
+      <c r="H40" s="17">
         <f>I56</f>
         <v>0.18325957145940461</v>
       </c>
-      <c r="I40" s="15">
+      <c r="I40" s="22">
         <f t="shared" ref="I40:I49" si="8">H13</f>
         <v>3.5999999999999997E-2</v>
       </c>
@@ -5096,15 +5110,15 @@
         <f t="shared" ref="F41:F49" si="9">J28</f>
         <v>21.432051577455791</v>
       </c>
-      <c r="G41" s="7">
+      <c r="G41" s="19">
         <f t="shared" ref="G41:G49" si="10">N28</f>
         <v>2.1991148575128552</v>
       </c>
-      <c r="H41" s="14">
+      <c r="H41" s="17">
         <f t="shared" ref="H41:H49" si="11">I57</f>
         <v>0.40317105721069013</v>
       </c>
-      <c r="I41" s="15">
+      <c r="I41" s="22">
         <f t="shared" si="8"/>
         <v>8.5499999999999993E-2</v>
       </c>
@@ -5114,15 +5128,15 @@
         <f t="shared" si="9"/>
         <v>38.78180761634858</v>
       </c>
-      <c r="G42" s="7">
+      <c r="G42" s="19">
         <f t="shared" si="10"/>
         <v>3.9793506945470711</v>
       </c>
-      <c r="H42" s="14">
+      <c r="H42" s="17">
         <f t="shared" si="11"/>
         <v>0.60213859193804364</v>
       </c>
-      <c r="I42" s="15">
+      <c r="I42" s="22">
         <f t="shared" si="8"/>
         <v>0.11249999999999999</v>
       </c>
@@ -5132,15 +5146,15 @@
         <f t="shared" si="9"/>
         <v>51.028694232037601</v>
       </c>
-      <c r="G43" s="7">
+      <c r="G43" s="19">
         <f t="shared" si="10"/>
         <v>5.2359877559829888</v>
       </c>
-      <c r="H43" s="14">
+      <c r="H43" s="17">
         <f t="shared" si="11"/>
         <v>0.79587013890941427</v>
       </c>
-      <c r="I43" s="15">
+      <c r="I43" s="22">
         <f t="shared" si="8"/>
         <v>0.13500000000000001</v>
       </c>
@@ -5150,15 +5164,15 @@
         <f t="shared" si="9"/>
         <v>62.255006963085876</v>
       </c>
-      <c r="G44" s="7">
+      <c r="G44" s="19">
         <f t="shared" si="10"/>
         <v>6.3879050622992457</v>
       </c>
-      <c r="H44" s="14">
+      <c r="H44" s="17">
         <f t="shared" si="11"/>
         <v>1.0053096491487339</v>
       </c>
-      <c r="I44" s="15">
+      <c r="I44" s="22">
         <f t="shared" si="8"/>
         <v>0.1575</v>
       </c>
@@ -5168,15 +5182,15 @@
         <f t="shared" si="9"/>
         <v>78.5841891173379</v>
       </c>
-      <c r="G45" s="7">
+      <c r="G45" s="19">
         <f t="shared" si="10"/>
         <v>8.0634211442138017</v>
       </c>
-      <c r="H45" s="14">
+      <c r="H45" s="17">
         <f t="shared" si="11"/>
         <v>1.2409290981679681</v>
       </c>
-      <c r="I45" s="15">
+      <c r="I45" s="22">
         <f t="shared" si="8"/>
         <v>0.18449999999999997</v>
       </c>
@@ -5186,15 +5200,15 @@
         <f t="shared" si="9"/>
         <v>84.707632425182425</v>
       </c>
-      <c r="G46" s="7">
+      <c r="G46" s="19">
         <f t="shared" si="10"/>
         <v>8.6917396749317621</v>
       </c>
-      <c r="H46" s="14">
+      <c r="H46" s="17">
         <f t="shared" si="11"/>
         <v>1.4241886696273729</v>
       </c>
-      <c r="I46" s="15">
+      <c r="I46" s="22">
         <f t="shared" si="8"/>
         <v>0.20249999999999999</v>
       </c>
@@ -5204,15 +5218,15 @@
         <f t="shared" si="9"/>
         <v>97.975092925512186</v>
       </c>
-      <c r="G47" s="7">
+      <c r="G47" s="19">
         <f t="shared" si="10"/>
         <v>10.053096491487338</v>
       </c>
-      <c r="H47" s="14">
+      <c r="H47" s="17">
         <f t="shared" si="11"/>
         <v>1.7383479349863522</v>
       </c>
-      <c r="I47" s="15">
+      <c r="I47" s="22">
         <f t="shared" si="8"/>
         <v>0.2475</v>
       </c>
@@ -5222,15 +5236,15 @@
         <f t="shared" si="9"/>
         <v>116.34542284904572</v>
       </c>
-      <c r="G48" s="7">
+      <c r="G48" s="19">
         <f t="shared" si="10"/>
         <v>11.938052083641214</v>
       </c>
-      <c r="H48" s="14">
+      <c r="H48" s="17">
         <f t="shared" si="11"/>
         <v>1.858775653373961</v>
       </c>
-      <c r="I48" s="15">
+      <c r="I48" s="22">
         <f t="shared" si="8"/>
         <v>0.25650000000000001</v>
       </c>
@@ -5240,428 +5254,437 @@
         <f t="shared" si="9"/>
         <v>120.42771838760873</v>
       </c>
-      <c r="G49" s="7">
+      <c r="G49" s="20">
         <f t="shared" si="10"/>
         <v>12.356931104119854</v>
       </c>
-      <c r="H49" s="16">
+      <c r="H49" s="17">
         <f t="shared" si="11"/>
         <v>1.9896753472735356</v>
       </c>
-      <c r="I49" s="17">
+      <c r="I49" s="23">
         <f t="shared" si="8"/>
         <v>0.27</v>
       </c>
     </row>
     <row r="54" spans="5:19" x14ac:dyDescent="0.35">
       <c r="E54" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="55" spans="5:19" x14ac:dyDescent="0.35">
+      <c r="E55" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G55" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H55" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I55" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="J55" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="K55" s="7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="55" spans="5:19" x14ac:dyDescent="0.35">
-      <c r="E55" t="s">
-        <v>10</v>
-      </c>
-      <c r="F55" t="s">
-        <v>43</v>
-      </c>
-      <c r="G55" t="s">
-        <v>48</v>
-      </c>
-      <c r="H55" t="s">
-        <v>44</v>
-      </c>
-      <c r="I55" t="s">
-        <v>45</v>
-      </c>
-      <c r="J55" t="s">
-        <v>46</v>
-      </c>
-      <c r="K55" t="s">
-        <v>47</v>
-      </c>
-      <c r="L55" s="18"/>
-      <c r="M55" s="18"/>
-      <c r="N55" s="18"/>
-      <c r="O55" s="18"/>
-      <c r="P55" s="18"/>
-      <c r="Q55" s="18"/>
-      <c r="R55" s="18"/>
-      <c r="S55" s="18"/>
+      <c r="L55" s="11"/>
+      <c r="M55" s="11"/>
+      <c r="N55" s="11"/>
+      <c r="O55" s="11"/>
+      <c r="P55" s="11"/>
+      <c r="Q55" s="11"/>
+      <c r="R55" s="11"/>
+      <c r="S55" s="11"/>
     </row>
     <row r="56" spans="5:19" x14ac:dyDescent="0.35">
-      <c r="E56">
+      <c r="E56" s="7">
         <v>0.5</v>
       </c>
-      <c r="F56">
+      <c r="F56" s="7">
         <v>0.04</v>
       </c>
-      <c r="G56">
+      <c r="G56" s="7">
         <f t="shared" ref="G56:G65" si="12">$B$21</f>
         <v>2.8</v>
       </c>
-      <c r="H56">
+      <c r="H56" s="7">
         <v>1.75</v>
       </c>
-      <c r="I56">
+      <c r="I56" s="7">
         <f>(H56*2*PI())/60</f>
         <v>0.18325957145940461</v>
       </c>
-      <c r="J56">
+      <c r="J56" s="7">
         <f>(E56-G56*F56)/I56</f>
         <v>2.1172154715310421</v>
       </c>
-      <c r="K56">
+      <c r="K56" s="7">
         <f>AVERAGE(J56:J65)</f>
         <v>2.2576395387322665</v>
       </c>
-      <c r="L56" s="18"/>
-      <c r="M56" s="18"/>
-      <c r="N56" s="18"/>
-      <c r="O56" s="18"/>
-      <c r="P56" s="18"/>
-      <c r="Q56" s="18"/>
-      <c r="R56" s="18"/>
-      <c r="S56" s="18"/>
+      <c r="L56" s="11"/>
+      <c r="M56" s="11"/>
+      <c r="N56" s="11"/>
+      <c r="O56" s="11"/>
+      <c r="P56" s="11"/>
+      <c r="Q56" s="11"/>
+      <c r="R56" s="11"/>
+      <c r="S56" s="11"/>
     </row>
     <row r="57" spans="5:19" x14ac:dyDescent="0.35">
-      <c r="E57">
+      <c r="E57" s="7">
         <v>1</v>
       </c>
-      <c r="F57">
+      <c r="F57" s="7">
         <v>4.7E-2</v>
       </c>
-      <c r="G57">
+      <c r="G57" s="7">
         <f t="shared" si="12"/>
         <v>2.8</v>
       </c>
-      <c r="H57">
+      <c r="H57" s="7">
         <v>3.85</v>
       </c>
-      <c r="I57">
+      <c r="I57" s="7">
         <f t="shared" ref="I57:I65" si="13">(H57*2*PI())/60</f>
         <v>0.40317105721069013</v>
       </c>
-      <c r="J57">
+      <c r="J57" s="7">
         <f t="shared" ref="J57:J65" si="14">(E57-G57*F57)/I57</f>
         <v>2.1539244558078221</v>
       </c>
-      <c r="L57" s="18"/>
-      <c r="M57" s="18"/>
-      <c r="N57" s="18"/>
-      <c r="O57" s="18"/>
-      <c r="P57" s="18"/>
-      <c r="Q57" s="18"/>
-      <c r="R57" s="18"/>
-      <c r="S57" s="18"/>
+      <c r="K57" s="7"/>
+      <c r="L57" s="11"/>
+      <c r="M57" s="11"/>
+      <c r="N57" s="11"/>
+      <c r="O57" s="11"/>
+      <c r="P57" s="11"/>
+      <c r="Q57" s="11"/>
+      <c r="R57" s="11"/>
+      <c r="S57" s="11"/>
     </row>
     <row r="58" spans="5:19" x14ac:dyDescent="0.35">
-      <c r="E58">
+      <c r="E58" s="7">
         <v>1.5</v>
       </c>
-      <c r="F58">
+      <c r="F58" s="7">
         <v>0.05</v>
       </c>
-      <c r="G58">
+      <c r="G58" s="7">
         <f t="shared" si="12"/>
         <v>2.8</v>
       </c>
-      <c r="H58">
+      <c r="H58" s="7">
         <v>5.75</v>
       </c>
-      <c r="I58">
+      <c r="I58" s="7">
         <f t="shared" si="13"/>
         <v>0.60213859193804364</v>
       </c>
-      <c r="J58">
+      <c r="J58" s="7">
         <f t="shared" si="14"/>
         <v>2.2586162358780282</v>
       </c>
-      <c r="L58" s="18"/>
-      <c r="M58" s="18"/>
-      <c r="N58" s="18"/>
-      <c r="O58" s="18"/>
-      <c r="P58" s="18"/>
-      <c r="Q58" s="18"/>
-      <c r="R58" s="18"/>
-      <c r="S58" s="18"/>
+      <c r="K58" s="7"/>
+      <c r="L58" s="11"/>
+      <c r="M58" s="11"/>
+      <c r="N58" s="11"/>
+      <c r="O58" s="11"/>
+      <c r="P58" s="11"/>
+      <c r="Q58" s="11"/>
+      <c r="R58" s="11"/>
+      <c r="S58" s="11"/>
     </row>
     <row r="59" spans="5:19" x14ac:dyDescent="0.35">
-      <c r="E59">
+      <c r="E59" s="7">
         <v>2</v>
       </c>
-      <c r="F59">
+      <c r="F59" s="7">
         <v>5.5E-2</v>
       </c>
-      <c r="G59">
+      <c r="G59" s="7">
         <f t="shared" si="12"/>
         <v>2.8</v>
       </c>
-      <c r="H59">
+      <c r="H59" s="7">
         <v>7.6</v>
       </c>
-      <c r="I59">
+      <c r="I59" s="7">
         <f t="shared" si="13"/>
         <v>0.79587013890941427</v>
       </c>
-      <c r="J59">
+      <c r="J59" s="7">
         <f t="shared" si="14"/>
         <v>2.3194738811655697</v>
       </c>
-      <c r="L59" s="18"/>
-      <c r="M59" s="18"/>
-      <c r="N59" s="18"/>
-      <c r="O59" s="18"/>
-      <c r="P59" s="18"/>
-      <c r="Q59" s="18"/>
-      <c r="R59" s="18"/>
-      <c r="S59" s="18"/>
+      <c r="K59" s="7"/>
+      <c r="L59" s="11"/>
+      <c r="M59" s="11"/>
+      <c r="N59" s="11"/>
+      <c r="O59" s="11"/>
+      <c r="P59" s="11"/>
+      <c r="Q59" s="11"/>
+      <c r="R59" s="11"/>
+      <c r="S59" s="11"/>
     </row>
     <row r="60" spans="5:19" x14ac:dyDescent="0.35">
-      <c r="E60">
+      <c r="E60" s="7">
         <v>2.5</v>
       </c>
-      <c r="F60">
+      <c r="F60" s="7">
         <v>0.06</v>
       </c>
-      <c r="G60">
+      <c r="G60" s="7">
         <f t="shared" si="12"/>
         <v>2.8</v>
       </c>
-      <c r="H60">
+      <c r="H60" s="7">
         <v>9.6</v>
       </c>
-      <c r="I60">
+      <c r="I60" s="7">
         <f t="shared" si="13"/>
         <v>1.0053096491487339</v>
       </c>
-      <c r="J60">
+      <c r="J60" s="7">
         <f t="shared" si="14"/>
         <v>2.3196832955643742</v>
       </c>
-      <c r="L60" s="18"/>
-      <c r="M60" s="18"/>
-      <c r="N60" s="18"/>
-      <c r="O60" s="18"/>
-      <c r="P60" s="18"/>
-      <c r="Q60" s="18"/>
-      <c r="R60" s="18"/>
-      <c r="S60" s="18"/>
+      <c r="K60" s="7"/>
+      <c r="L60" s="11"/>
+      <c r="M60" s="11"/>
+      <c r="N60" s="11"/>
+      <c r="O60" s="11"/>
+      <c r="P60" s="11"/>
+      <c r="Q60" s="11"/>
+      <c r="R60" s="11"/>
+      <c r="S60" s="11"/>
     </row>
     <row r="61" spans="5:19" x14ac:dyDescent="0.35">
-      <c r="E61">
+      <c r="E61" s="7">
         <v>3</v>
       </c>
-      <c r="F61">
+      <c r="F61" s="7">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="G61">
+      <c r="G61" s="7">
         <f t="shared" si="12"/>
         <v>2.8</v>
       </c>
-      <c r="H61">
+      <c r="H61" s="7">
         <v>11.85</v>
       </c>
-      <c r="I61">
+      <c r="I61" s="7">
         <f t="shared" si="13"/>
         <v>1.2409290981679681</v>
       </c>
-      <c r="J61">
+      <c r="J61" s="7">
         <f t="shared" si="14"/>
         <v>2.2708791373820816</v>
       </c>
-      <c r="L61" s="18"/>
-      <c r="M61" s="18"/>
-      <c r="N61" s="18"/>
-      <c r="O61" s="18"/>
-      <c r="P61" s="18"/>
-      <c r="Q61" s="18"/>
-      <c r="R61" s="18"/>
-      <c r="S61" s="18"/>
+      <c r="K61" s="7"/>
+      <c r="L61" s="11"/>
+      <c r="M61" s="11"/>
+      <c r="N61" s="11"/>
+      <c r="O61" s="11"/>
+      <c r="P61" s="11"/>
+      <c r="Q61" s="11"/>
+      <c r="R61" s="11"/>
+      <c r="S61" s="11"/>
     </row>
     <row r="62" spans="5:19" x14ac:dyDescent="0.35">
-      <c r="E62">
+      <c r="E62" s="7">
         <v>3.5</v>
       </c>
-      <c r="F62">
+      <c r="F62" s="7">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="G62">
+      <c r="G62" s="7">
         <f t="shared" si="12"/>
         <v>2.8</v>
       </c>
-      <c r="H62">
+      <c r="H62" s="7">
         <v>13.6</v>
       </c>
-      <c r="I62">
+      <c r="I62" s="7">
         <f t="shared" si="13"/>
         <v>1.4241886696273729</v>
       </c>
-      <c r="J62">
+      <c r="J62" s="7">
         <f t="shared" si="14"/>
         <v>2.3218833786012332</v>
       </c>
-      <c r="L62" s="18"/>
-      <c r="M62" s="18"/>
-      <c r="N62" s="18"/>
-      <c r="O62" s="18"/>
-      <c r="P62" s="18"/>
-      <c r="Q62" s="18"/>
-      <c r="R62" s="18"/>
-      <c r="S62" s="18"/>
+      <c r="K62" s="7"/>
+      <c r="L62" s="11"/>
+      <c r="M62" s="11"/>
+      <c r="N62" s="11"/>
+      <c r="O62" s="11"/>
+      <c r="P62" s="11"/>
+      <c r="Q62" s="11"/>
+      <c r="R62" s="11"/>
+      <c r="S62" s="11"/>
     </row>
     <row r="63" spans="5:19" x14ac:dyDescent="0.35">
-      <c r="E63">
+      <c r="E63" s="7">
         <v>4</v>
       </c>
-      <c r="F63">
+      <c r="F63" s="7">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="G63">
+      <c r="G63" s="7">
         <f t="shared" si="12"/>
         <v>2.8</v>
       </c>
-      <c r="H63">
+      <c r="H63" s="7">
         <v>16.600000000000001</v>
       </c>
-      <c r="I63">
+      <c r="I63" s="7">
         <f t="shared" si="13"/>
         <v>1.7383479349863522</v>
       </c>
-      <c r="J63">
+      <c r="J63" s="7">
         <f t="shared" si="14"/>
         <v>2.167345169613343</v>
       </c>
-      <c r="L63" s="18"/>
-      <c r="M63" s="18"/>
-      <c r="N63" s="18"/>
-      <c r="O63" s="18"/>
-      <c r="P63" s="18"/>
-      <c r="Q63" s="18"/>
-      <c r="R63" s="18"/>
-      <c r="S63" s="18"/>
+      <c r="K63" s="7"/>
+      <c r="L63" s="11"/>
+      <c r="M63" s="11"/>
+      <c r="N63" s="11"/>
+      <c r="O63" s="11"/>
+      <c r="P63" s="11"/>
+      <c r="Q63" s="11"/>
+      <c r="R63" s="11"/>
+      <c r="S63" s="11"/>
     </row>
     <row r="64" spans="5:19" x14ac:dyDescent="0.35">
-      <c r="E64">
+      <c r="E64" s="7">
         <v>4.5</v>
       </c>
-      <c r="F64">
+      <c r="F64" s="7">
         <v>9.4E-2</v>
       </c>
-      <c r="G64">
+      <c r="G64" s="7">
         <f t="shared" si="12"/>
         <v>2.8</v>
       </c>
-      <c r="H64">
+      <c r="H64" s="7">
         <v>17.75</v>
       </c>
-      <c r="I64">
+      <c r="I64" s="7">
         <f t="shared" si="13"/>
         <v>1.858775653373961</v>
       </c>
-      <c r="J64">
+      <c r="J64" s="7">
         <f t="shared" si="14"/>
         <v>2.2793498463946213</v>
       </c>
-      <c r="L64" s="18"/>
-      <c r="M64" s="18"/>
-      <c r="N64" s="18"/>
-      <c r="O64" s="18"/>
-      <c r="P64" s="18"/>
-      <c r="Q64" s="18"/>
-      <c r="R64" s="18"/>
-      <c r="S64" s="18"/>
+      <c r="K64" s="7"/>
+      <c r="L64" s="11"/>
+      <c r="M64" s="11"/>
+      <c r="N64" s="11"/>
+      <c r="O64" s="11"/>
+      <c r="P64" s="11"/>
+      <c r="Q64" s="11"/>
+      <c r="R64" s="11"/>
+      <c r="S64" s="11"/>
     </row>
     <row r="65" spans="5:19" x14ac:dyDescent="0.35">
-      <c r="E65">
+      <c r="E65" s="7">
         <v>5</v>
       </c>
-      <c r="F65">
+      <c r="F65" s="7">
         <v>0.10299999999999999</v>
       </c>
-      <c r="G65">
+      <c r="G65" s="7">
         <f t="shared" si="12"/>
         <v>2.8</v>
       </c>
-      <c r="H65">
+      <c r="H65" s="7">
         <v>19</v>
       </c>
-      <c r="I65">
-        <f t="shared" si="13"/>
+      <c r="I65" s="7">
+        <f>(H65*2*PI())/60</f>
         <v>1.9896753472735356</v>
       </c>
-      <c r="J65">
+      <c r="J65" s="7">
         <f t="shared" si="14"/>
         <v>2.3680245153845498</v>
       </c>
-      <c r="L65" s="18"/>
-      <c r="M65" s="18"/>
-      <c r="N65" s="18"/>
-      <c r="O65" s="18"/>
-      <c r="P65" s="18"/>
-      <c r="Q65" s="18"/>
-      <c r="R65" s="18"/>
-      <c r="S65" s="18"/>
+      <c r="K65" s="7"/>
+      <c r="L65" s="11"/>
+      <c r="M65" s="11"/>
+      <c r="N65" s="11"/>
+      <c r="O65" s="11"/>
+      <c r="P65" s="11"/>
+      <c r="Q65" s="11"/>
+      <c r="R65" s="11"/>
+      <c r="S65" s="11"/>
     </row>
     <row r="66" spans="5:19" x14ac:dyDescent="0.35">
-      <c r="L66" s="18"/>
-      <c r="M66" s="18"/>
-      <c r="N66" s="18"/>
-      <c r="O66" s="18"/>
-      <c r="P66" s="18"/>
-      <c r="Q66" s="18"/>
-      <c r="R66" s="18"/>
-      <c r="S66" s="18"/>
+      <c r="L66" s="11"/>
+      <c r="M66" s="11"/>
+      <c r="N66" s="11"/>
+      <c r="O66" s="11"/>
+      <c r="P66" s="11"/>
+      <c r="Q66" s="11"/>
+      <c r="R66" s="11"/>
+      <c r="S66" s="11"/>
     </row>
     <row r="67" spans="5:19" x14ac:dyDescent="0.35">
-      <c r="L67" s="18"/>
-      <c r="M67" s="18"/>
-      <c r="N67" s="18"/>
-      <c r="O67" s="18"/>
-      <c r="P67" s="18"/>
-      <c r="Q67" s="18"/>
-      <c r="R67" s="18"/>
-      <c r="S67" s="18"/>
+      <c r="L67" s="11"/>
+      <c r="M67" s="11"/>
+      <c r="N67" s="11"/>
+      <c r="O67" s="11"/>
+      <c r="P67" s="11"/>
+      <c r="Q67" s="11"/>
+      <c r="R67" s="11"/>
+      <c r="S67" s="11"/>
     </row>
     <row r="68" spans="5:19" x14ac:dyDescent="0.35">
-      <c r="L68" s="18"/>
-      <c r="M68" s="18"/>
-      <c r="N68" s="18"/>
-      <c r="O68" s="18"/>
-      <c r="P68" s="18"/>
-      <c r="Q68" s="18"/>
-      <c r="R68" s="18"/>
-      <c r="S68" s="18"/>
+      <c r="L68" s="11"/>
+      <c r="M68" s="11"/>
+      <c r="N68" s="11"/>
+      <c r="O68" s="11"/>
+      <c r="P68" s="11"/>
+      <c r="Q68" s="11"/>
+      <c r="R68" s="11"/>
+      <c r="S68" s="11"/>
     </row>
     <row r="69" spans="5:19" x14ac:dyDescent="0.35">
-      <c r="L69" s="18"/>
-      <c r="M69" s="18"/>
-      <c r="N69" s="18"/>
-      <c r="O69" s="18"/>
-      <c r="P69" s="18"/>
-      <c r="Q69" s="18"/>
-      <c r="R69" s="18"/>
-      <c r="S69" s="18"/>
+      <c r="L69" s="11"/>
+      <c r="M69" s="11"/>
+      <c r="N69" s="11"/>
+      <c r="O69" s="11"/>
+      <c r="P69" s="11"/>
+      <c r="Q69" s="11"/>
+      <c r="R69" s="11"/>
+      <c r="S69" s="11"/>
     </row>
     <row r="70" spans="5:19" x14ac:dyDescent="0.35">
-      <c r="L70" s="18"/>
-      <c r="M70" s="18"/>
-      <c r="N70" s="18"/>
-      <c r="O70" s="18"/>
-      <c r="P70" s="18"/>
-      <c r="Q70" s="18"/>
-      <c r="R70" s="18"/>
-      <c r="S70" s="18"/>
+      <c r="L70" s="11"/>
+      <c r="M70" s="11"/>
+      <c r="N70" s="11"/>
+      <c r="O70" s="11"/>
+      <c r="P70" s="11"/>
+      <c r="Q70" s="11"/>
+      <c r="R70" s="11"/>
+      <c r="S70" s="11"/>
     </row>
     <row r="71" spans="5:19" x14ac:dyDescent="0.35">
-      <c r="L71" s="18"/>
-      <c r="M71" s="18"/>
-      <c r="N71" s="18"/>
-      <c r="O71" s="18"/>
-      <c r="P71" s="18"/>
-      <c r="Q71" s="18"/>
-      <c r="R71" s="18"/>
-      <c r="S71" s="18"/>
+      <c r="L71" s="11"/>
+      <c r="M71" s="11"/>
+      <c r="N71" s="11"/>
+      <c r="O71" s="11"/>
+      <c r="P71" s="11"/>
+      <c r="Q71" s="11"/>
+      <c r="R71" s="11"/>
+      <c r="S71" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>